<commit_message>
Added Selection Test project. Fixed loads of bugs.
</commit_message>
<xml_diff>
--- a/CsvXlsImportUnitTests/Data/XlsImport1.xlsx
+++ b/CsvXlsImportUnitTests/Data/XlsImport1.xlsx
@@ -889,7 +889,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -944,7 +946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>